<commit_message>
Update comparison with FEM data
</commit_message>
<xml_diff>
--- a/validation/elephant_trunk/number_of_modes.xlsx
+++ b/validation/elephant_trunk/number_of_modes.xlsx
@@ -15,29 +15,22 @@
     <sheet name="resonances" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">resonances!$A$3:$A$5</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">resonances!$B$10:$Q$10</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">resonances!$B$15:$Q$15</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">resonances!$B$16:$Q$16</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">resonances!$B$17:$Q$17</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">resonances!$B$33:$Q$33</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">resonances!$B$34:$Q$34</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">resonances!$B$35:$Q$35</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">resonances!$B$8:$Q$8</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">resonances!$B$9:$Q$9</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">resonances!$B$52:$Q$52</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">resonances!$B$53:$Q$53</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">resonances!$B$54:$Q$54</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">resonances!$B$52:$Q$52</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">resonances!$B$53:$Q$53</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">resonances!$B$54:$Q$54</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">resonances!$B$33:$Q$33</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">resonances!$B$34:$Q$34</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">resonances!$B$35:$Q$35</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">resonances!$B$15:$Q$15</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">resonances!$B$16:$Q$16</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">resonances!$B$17:$Q$17</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">resonances!$B$52:$Q$52</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">resonances!$B$53:$Q$53</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">resonances!$B$54:$Q$54</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="28">
   <si>
     <t>Frequencies</t>
   </si>
@@ -115,6 +108,12 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>Max 8kHz</t>
+  </si>
+  <si>
+    <t>Average 8kHz</t>
   </si>
 </sst>
 </file>
@@ -638,17 +637,17 @@
     <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -712,17 +711,17 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.10</cx:f>
+        <cx:f dir="row">_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.11</cx:f>
+        <cx:f dir="row">_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.12</cx:f>
+        <cx:f dir="row">_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -771,17 +770,17 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.13</cx:f>
+        <cx:f dir="row">_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.14</cx:f>
+        <cx:f dir="row">_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.15</cx:f>
+        <cx:f dir="row">_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -830,17 +829,17 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.4</cx:f>
+        <cx:f dir="row">_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.5</cx:f>
+        <cx:f dir="row">_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.6</cx:f>
+        <cx:f dir="row">_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2936,8 +2935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="O55" sqref="O55"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="S58" sqref="S58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3275,7 +3274,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="3">
@@ -3352,7 +3351,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="3">
         <f>100*ABS(B6-B4)/B6</f>
         <v>0.11198208286674133</v>
@@ -3427,7 +3426,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="3">
         <f>100*ABS(B6-B5)/B6</f>
         <v>0.11198208286674133</v>
@@ -3502,7 +3501,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="2">
@@ -3576,7 +3575,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="2">
         <f>100*ABS(B7-B4)/B7</f>
         <v>0.11173184357541899</v>
@@ -3648,7 +3647,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="2">
         <f>100*ABS(B7-B5)/B7</f>
         <v>0.11173184357541899</v>
@@ -3720,7 +3719,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="2">
         <f>100*ABS(B7-B6)/B7</f>
         <v>0.22346368715083798</v>
@@ -3792,205 +3791,215 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7">
         <f>LOG(B8)</f>
         <v>-0.64982146322456524</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="7">
         <f t="shared" ref="C15:Q15" si="9">LOG(C8)</f>
         <v>-0.7512791039833423</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="7">
         <f t="shared" si="9"/>
         <v>-0.81607550709726973</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="7">
         <f t="shared" si="9"/>
         <v>-0.85418454383360665</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="7">
         <f t="shared" si="9"/>
         <v>-1.1733805401587045</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="7">
         <f t="shared" si="9"/>
         <v>-1.1805081766692895</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="7">
         <f t="shared" si="9"/>
         <v>-0.88994166501946403</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="7">
         <f t="shared" si="9"/>
         <v>-0.80881093086028999</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="7">
         <f t="shared" si="9"/>
         <v>-0.89941008077244988</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K15" s="7">
         <f t="shared" si="9"/>
         <v>-0.7280414522832771</v>
       </c>
-      <c r="L15" s="9">
+      <c r="L15" s="7">
         <f t="shared" si="9"/>
         <v>-0.86039790512731285</v>
       </c>
-      <c r="M15" s="9">
+      <c r="M15" s="7">
         <f t="shared" si="9"/>
         <v>-1.6084725457414342</v>
       </c>
-      <c r="N15" s="9">
+      <c r="N15" s="7">
         <f t="shared" si="9"/>
         <v>3.9514808204530377E-2</v>
       </c>
-      <c r="O15" s="9">
+      <c r="O15" s="7">
         <f t="shared" si="9"/>
         <v>0.40972819922774567</v>
       </c>
-      <c r="P15" s="9">
+      <c r="P15" s="7">
         <f t="shared" si="9"/>
         <v>0.68844520947853827</v>
       </c>
-      <c r="Q15" s="9">
+      <c r="Q15" s="7">
         <f t="shared" si="9"/>
         <v>-0.51982799377571876</v>
       </c>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
+      <c r="R15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S15" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7">
         <f t="shared" ref="B16:Q16" si="10">LOG(B9)</f>
         <v>-0.95085145888854639</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="7">
         <f t="shared" si="10"/>
         <v>-1.2284003587030048</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="7">
         <f t="shared" si="10"/>
         <v>-1.1171055027612509</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="7">
         <f t="shared" si="10"/>
         <v>-1.2521245525056441</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="7">
         <f t="shared" si="10"/>
         <v>-1.6505017948783669</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="7">
         <f t="shared" si="10"/>
         <v>-1.6576294313889519</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="7">
         <f t="shared" si="10"/>
         <v>-1.2579184503140584</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="7">
         <f t="shared" si="10"/>
         <v>-1.2859321855799524</v>
       </c>
-      <c r="J16" s="9">
+      <c r="J16" s="7">
         <f t="shared" si="10"/>
         <v>-1.2004400764364311</v>
       </c>
-      <c r="K16" s="9">
+      <c r="K16" s="7">
         <f t="shared" si="10"/>
         <v>-1.1430148002540952</v>
       </c>
-      <c r="L16" s="9">
+      <c r="L16" s="7">
         <f t="shared" si="10"/>
         <v>-1.2583379137993504</v>
       </c>
-      <c r="M16" s="9">
+      <c r="M16" s="7">
         <f t="shared" si="10"/>
         <v>-1.6084725457414342</v>
       </c>
-      <c r="N16" s="9">
+      <c r="N16" s="7">
         <f t="shared" si="10"/>
         <v>-1.2571503820570007</v>
       </c>
-      <c r="O16" s="9">
+      <c r="O16" s="7">
         <f t="shared" si="10"/>
         <v>-1.3666097103924297</v>
       </c>
-      <c r="P16" s="9">
+      <c r="P16" s="7">
         <f t="shared" si="10"/>
         <v>-1.1467922639217683</v>
       </c>
-      <c r="Q16" s="9">
+      <c r="Q16" s="7">
         <f t="shared" si="10"/>
         <v>-1.2979792441593623</v>
       </c>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
+      <c r="R16" s="8">
+        <f>MAX(B14:L14)</f>
+        <v>0.22346368715083798</v>
+      </c>
+      <c r="S16" s="8">
+        <f>AVERAGE(B14:L14)</f>
+        <v>0.10344890744178456</v>
+      </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="9">
+      <c r="B17" s="7">
         <f t="shared" ref="B17:Q17" si="11">LOG(B10)</f>
         <v>-0.95085145888854639</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="7">
         <f t="shared" si="11"/>
         <v>-1.2284003587030048</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="7">
         <f t="shared" si="11"/>
         <v>-1.4181354984252321</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="7">
         <f t="shared" si="11"/>
         <v>-1.5531545481696254</v>
       </c>
-      <c r="F17" s="9" t="e">
+      <c r="F17" s="7" t="e">
         <f t="shared" si="11"/>
         <v>#NUM!</v>
       </c>
-      <c r="G17" s="9" t="e">
+      <c r="G17" s="7" t="e">
         <f t="shared" si="11"/>
         <v>#NUM!</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="7">
         <f t="shared" si="11"/>
         <v>-1.7350397050337207</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17" s="7">
         <f t="shared" si="11"/>
         <v>-1.7630534402996147</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="7">
         <f t="shared" si="11"/>
         <v>-1.5014700721004122</v>
       </c>
-      <c r="K17" s="9">
+      <c r="K17" s="7">
         <f t="shared" si="11"/>
         <v>-1.5409548089261327</v>
       </c>
-      <c r="L17" s="9">
+      <c r="L17" s="7">
         <f t="shared" si="11"/>
         <v>-1.5593679094633317</v>
       </c>
-      <c r="M17" s="9" t="e">
+      <c r="M17" s="7" t="e">
         <f t="shared" si="11"/>
         <v>#NUM!</v>
       </c>
-      <c r="N17" s="9">
+      <c r="N17" s="7">
         <f t="shared" si="11"/>
         <v>-1.6550903907290384</v>
       </c>
-      <c r="O17" s="9">
+      <c r="O17" s="7">
         <f t="shared" si="11"/>
         <v>-1.968669701720392</v>
       </c>
-      <c r="P17" s="9">
+      <c r="P17" s="7">
         <f t="shared" si="11"/>
         <v>-1.6908603082720439</v>
       </c>
-      <c r="Q17" s="9">
+      <c r="Q17" s="7">
         <f t="shared" si="11"/>
         <v>-1.6959192528314</v>
       </c>
@@ -4325,7 +4334,7 @@
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B26" s="3">
@@ -4402,7 +4411,7 @@
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
+      <c r="A27" s="10"/>
       <c r="B27" s="3">
         <f>100*ABS(B24-B22)/B24</f>
         <v>0</v>
@@ -4477,7 +4486,7 @@
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
+      <c r="A28" s="10"/>
       <c r="B28" s="3">
         <f>100*ABS(B24-B23)/B24</f>
         <v>0</v>
@@ -4552,7 +4561,7 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B29" s="2">
@@ -4626,7 +4635,7 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="2">
         <f>100*ABS(B25-B22)/B25</f>
         <v>0</v>
@@ -4698,7 +4707,7 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="2">
         <f>100*ABS(B25-B23)/B25</f>
         <v>0</v>
@@ -4770,7 +4779,7 @@
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="2">
         <f>100*ABS(B25-B24)/B25</f>
         <v>0</v>
@@ -4842,205 +4851,215 @@
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="9" t="e">
+      <c r="A33" s="6"/>
+      <c r="B33" s="7" t="e">
         <f>LOG(B26)</f>
         <v>#NUM!</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33" s="7">
         <f t="shared" ref="C33:Q33" si="25">LOG(C26)</f>
         <v>0.34678748622465633</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D33" s="7">
         <f t="shared" si="25"/>
         <v>0.40893539297350084</v>
       </c>
-      <c r="E33" s="9" t="e">
+      <c r="E33" s="7" t="e">
         <f t="shared" si="25"/>
         <v>#NUM!</v>
       </c>
-      <c r="F33" s="9">
+      <c r="F33" s="7">
         <f t="shared" si="25"/>
         <v>0.85387196432176204</v>
       </c>
-      <c r="G33" s="9" t="e">
+      <c r="G33" s="7" t="e">
         <f t="shared" si="25"/>
         <v>#NUM!</v>
       </c>
-      <c r="H33" s="9">
+      <c r="H33" s="7">
         <f t="shared" si="25"/>
         <v>0.43179827593300502</v>
       </c>
-      <c r="I33" s="9" t="e">
+      <c r="I33" s="7" t="e">
         <f t="shared" si="25"/>
         <v>#NUM!</v>
       </c>
-      <c r="J33" s="9" t="e">
+      <c r="J33" s="7" t="e">
         <f t="shared" si="25"/>
         <v>#NUM!</v>
       </c>
-      <c r="K33" s="9">
+      <c r="K33" s="7">
         <f t="shared" si="25"/>
         <v>1.5056767151727153</v>
       </c>
-      <c r="L33" s="9">
+      <c r="L33" s="7">
         <f t="shared" si="25"/>
         <v>0.43179827593300502</v>
       </c>
-      <c r="M33" s="9">
+      <c r="M33" s="7">
         <f t="shared" si="25"/>
         <v>1.4616090885414148</v>
       </c>
-      <c r="N33" s="9">
+      <c r="N33" s="7">
         <f t="shared" si="25"/>
         <v>1.2768963159472619</v>
       </c>
-      <c r="O33" s="9">
+      <c r="O33" s="7">
         <f t="shared" si="25"/>
         <v>0.40893539297350084</v>
       </c>
-      <c r="P33" s="9">
+      <c r="P33" s="7">
         <f t="shared" si="25"/>
         <v>1.0555173278498313</v>
       </c>
-      <c r="Q33" s="9">
+      <c r="Q33" s="7">
         <f t="shared" si="25"/>
         <v>1.1079053973095196</v>
       </c>
-      <c r="R33" s="9"/>
-      <c r="S33" s="9"/>
+      <c r="R33" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S33" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="9" t="e">
+      <c r="A34" s="6"/>
+      <c r="B34" s="7" t="e">
         <f t="shared" ref="B34:Q35" si="26">LOG(B27)</f>
         <v>#NUM!</v>
       </c>
-      <c r="C34" s="9" t="e">
+      <c r="C34" s="7" t="e">
         <f t="shared" si="26"/>
         <v>#NUM!</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D34" s="7">
         <f t="shared" si="26"/>
         <v>0.40893539297350084</v>
       </c>
-      <c r="E34" s="9" t="e">
+      <c r="E34" s="7" t="e">
         <f t="shared" si="26"/>
         <v>#NUM!</v>
       </c>
-      <c r="F34" s="9">
+      <c r="F34" s="7">
         <f t="shared" si="26"/>
         <v>0.37675070960209955</v>
       </c>
-      <c r="G34" s="9" t="e">
+      <c r="G34" s="7" t="e">
         <f t="shared" si="26"/>
         <v>#NUM!</v>
       </c>
-      <c r="H34" s="9" t="e">
+      <c r="H34" s="7" t="e">
         <f t="shared" si="26"/>
         <v>#NUM!</v>
       </c>
-      <c r="I34" s="9">
+      <c r="I34" s="7">
         <f t="shared" si="26"/>
         <v>0.50863830616572725</v>
       </c>
-      <c r="J34" s="9">
+      <c r="J34" s="7">
         <f t="shared" si="26"/>
         <v>0.43179827593300502</v>
       </c>
-      <c r="K34" s="9">
+      <c r="K34" s="7">
         <f t="shared" si="26"/>
         <v>0.46428403001449026</v>
       </c>
-      <c r="L34" s="9" t="e">
+      <c r="L34" s="7" t="e">
         <f t="shared" si="26"/>
         <v>#NUM!</v>
       </c>
-      <c r="M34" s="9">
+      <c r="M34" s="7">
         <f t="shared" si="26"/>
         <v>0.89733765810285226</v>
       </c>
-      <c r="N34" s="9" t="e">
+      <c r="N34" s="7" t="e">
         <f t="shared" si="26"/>
         <v>#NUM!</v>
       </c>
-      <c r="O34" s="9">
+      <c r="O34" s="7">
         <f t="shared" si="26"/>
         <v>0.40893539297350084</v>
       </c>
-      <c r="P34" s="9" t="e">
+      <c r="P34" s="7" t="e">
         <f t="shared" si="26"/>
         <v>#NUM!</v>
       </c>
-      <c r="Q34" s="9" t="e">
+      <c r="Q34" s="7" t="e">
         <f t="shared" si="26"/>
         <v>#NUM!</v>
       </c>
-      <c r="R34" s="9"/>
-      <c r="S34" s="9"/>
+      <c r="R34" s="8">
+        <f>MAX(B32:L32)</f>
+        <v>21.276595744680851</v>
+      </c>
+      <c r="S34" s="8">
+        <f>AVERAGE(B32:L32)</f>
+        <v>6.7802506722474121</v>
+      </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B35" s="9" t="e">
+      <c r="B35" s="7" t="e">
         <f t="shared" si="26"/>
         <v>#NUM!</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35" s="7">
         <f t="shared" si="26"/>
         <v>0.34678748622465633</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D35" s="7">
         <f t="shared" si="26"/>
         <v>0.40893539297350084</v>
       </c>
-      <c r="E35" s="9">
+      <c r="E35" s="7">
         <f t="shared" si="26"/>
         <v>0.43179827593300502</v>
       </c>
-      <c r="F35" s="9">
+      <c r="F35" s="7">
         <f t="shared" si="26"/>
         <v>0.37675070960209955</v>
       </c>
-      <c r="G35" s="9" t="e">
+      <c r="G35" s="7" t="e">
         <f t="shared" si="26"/>
         <v>#NUM!</v>
       </c>
-      <c r="H35" s="9">
+      <c r="H35" s="7">
         <f t="shared" si="26"/>
         <v>0.43179827593300502</v>
       </c>
-      <c r="I35" s="9">
+      <c r="I35" s="7">
         <f t="shared" si="26"/>
         <v>0.20760831050174611</v>
       </c>
-      <c r="J35" s="9" t="e">
+      <c r="J35" s="7" t="e">
         <f t="shared" si="26"/>
         <v>#NUM!</v>
       </c>
-      <c r="K35" s="9" t="e">
+      <c r="K35" s="7" t="e">
         <f t="shared" si="26"/>
         <v>#NUM!</v>
       </c>
-      <c r="L35" s="9" t="e">
+      <c r="L35" s="7" t="e">
         <f t="shared" si="26"/>
         <v>#NUM!</v>
       </c>
-      <c r="M35" s="9">
+      <c r="M35" s="7">
         <f t="shared" si="26"/>
         <v>0.42021640338318988</v>
       </c>
-      <c r="N35" s="9" t="e">
+      <c r="N35" s="7" t="e">
         <f t="shared" si="26"/>
         <v>#NUM!</v>
       </c>
-      <c r="O35" s="9">
+      <c r="O35" s="7">
         <f t="shared" si="26"/>
         <v>0.40893539297350084</v>
       </c>
-      <c r="P35" s="9" t="e">
+      <c r="P35" s="7" t="e">
         <f t="shared" si="26"/>
         <v>#NUM!</v>
       </c>
-      <c r="Q35" s="9" t="e">
+      <c r="Q35" s="7" t="e">
         <f t="shared" si="26"/>
         <v>#NUM!</v>
       </c>
@@ -5375,7 +5394,7 @@
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B45" s="3">
@@ -5452,7 +5471,7 @@
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
+      <c r="A46" s="10"/>
       <c r="B46" s="3">
         <f>100*ABS(B43-B41)/B43</f>
         <v>2.8448403401684169E-2</v>
@@ -5527,7 +5546,7 @@
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
+      <c r="A47" s="10"/>
       <c r="B47" s="3">
         <f>100*ABS(B43-B42)/B43</f>
         <v>5.2794357267135779E-2</v>
@@ -5602,7 +5621,7 @@
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B48" s="2">
@@ -5676,7 +5695,7 @@
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
+      <c r="A49" s="9"/>
       <c r="B49" s="2">
         <f>100*ABS(B44-B41)/B44</f>
         <v>0.26806183557215724</v>
@@ -5748,7 +5767,7 @@
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
+      <c r="A50" s="9"/>
       <c r="B50" s="2">
         <f>100*ABS(B44-B42)/B44</f>
         <v>0.18701379886642444</v>
@@ -5820,7 +5839,7 @@
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
+      <c r="A51" s="9"/>
       <c r="B51" s="2">
         <f>100*ABS(B44-B43)/B44</f>
         <v>0.23968161776397426</v>
@@ -5892,199 +5911,213 @@
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B52" s="9">
+      <c r="B52" s="7">
         <f>LOG(B45)</f>
         <v>-0.98334845832901741</v>
       </c>
-      <c r="C52" s="9">
+      <c r="C52" s="7">
         <f t="shared" ref="C52:Q52" si="40">LOG(C45)</f>
         <v>-1.0389578955058087</v>
       </c>
-      <c r="D52" s="9">
+      <c r="D52" s="7">
         <f t="shared" si="40"/>
         <v>-1.0560076081483187</v>
       </c>
-      <c r="E52" s="9">
+      <c r="E52" s="7">
         <f t="shared" si="40"/>
         <v>-1.1408644620246871</v>
       </c>
-      <c r="F52" s="9">
+      <c r="F52" s="7">
         <f t="shared" si="40"/>
         <v>-0.43053531093245534</v>
       </c>
-      <c r="G52" s="9">
+      <c r="G52" s="7">
         <f t="shared" si="40"/>
         <v>-0.59300722555531127</v>
       </c>
-      <c r="H52" s="9">
+      <c r="H52" s="7">
         <f t="shared" si="40"/>
         <v>-2.2197370702949928</v>
       </c>
-      <c r="I52" s="9">
+      <c r="I52" s="7">
         <f t="shared" si="40"/>
         <v>-1.6523988918851396</v>
       </c>
-      <c r="J52" s="9">
+      <c r="J52" s="7">
         <f t="shared" si="40"/>
         <v>-1.2054114464083456</v>
       </c>
-      <c r="K52" s="9">
+      <c r="K52" s="7">
         <f t="shared" si="40"/>
         <v>-0.15931897411983356</v>
       </c>
-      <c r="L52" s="9">
+      <c r="L52" s="7">
         <f t="shared" si="40"/>
         <v>-1.0517614490297977</v>
       </c>
-      <c r="M52" s="9">
+      <c r="M52" s="7">
         <f t="shared" si="40"/>
         <v>0.30804778442963882</v>
       </c>
-      <c r="N52" s="9">
+      <c r="N52" s="7">
         <f t="shared" si="40"/>
         <v>0.80391224973878961</v>
       </c>
-      <c r="O52" s="9">
+      <c r="O52" s="7">
         <f t="shared" si="40"/>
         <v>0.76896517202994874</v>
       </c>
-      <c r="P52" s="9">
+      <c r="P52" s="7">
         <f t="shared" si="40"/>
         <v>0.70267102701037576</v>
       </c>
-      <c r="Q52" s="9">
+      <c r="Q52" s="7">
         <f t="shared" si="40"/>
         <v>0.80715669620779418</v>
       </c>
+      <c r="R52" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S52" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B53" s="9">
+      <c r="B53" s="7">
         <f t="shared" ref="B53:Q54" si="41">LOG(B46)</f>
         <v>-1.5459421023197202</v>
       </c>
-      <c r="C53" s="9">
+      <c r="C53" s="7">
         <f t="shared" si="41"/>
         <v>-1.5535786917208025</v>
       </c>
-      <c r="D53" s="9">
+      <c r="D53" s="7">
         <f t="shared" si="41"/>
         <v>-1.6853580394866405</v>
       </c>
-      <c r="E53" s="9">
+      <c r="E53" s="7">
         <f t="shared" si="41"/>
         <v>-1.7133666904989568</v>
       </c>
-      <c r="F53" s="9">
+      <c r="F53" s="7">
         <f t="shared" si="41"/>
         <v>-0.75090190106633814</v>
       </c>
-      <c r="G53" s="9">
+      <c r="G53" s="7">
         <f t="shared" si="41"/>
         <v>-1.1222685628684042</v>
       </c>
-      <c r="H53" s="9">
+      <c r="H53" s="7">
         <f t="shared" si="41"/>
         <v>-2.3672757313802681</v>
       </c>
-      <c r="I53" s="9">
+      <c r="I53" s="7">
         <f t="shared" si="41"/>
         <v>-1.1435473749348841</v>
       </c>
-      <c r="J53" s="9">
+      <c r="J53" s="7">
         <f t="shared" si="41"/>
         <v>-1.642921593674618</v>
       </c>
-      <c r="K53" s="9">
+      <c r="K53" s="7">
         <f t="shared" si="41"/>
         <v>-1.7048319006670909</v>
       </c>
-      <c r="L53" s="9">
+      <c r="L53" s="7">
         <f t="shared" si="41"/>
         <v>-1.1606578864294068</v>
       </c>
-      <c r="M53" s="9">
+      <c r="M53" s="7">
         <f t="shared" si="41"/>
         <v>-0.54615449419532358</v>
       </c>
-      <c r="N53" s="9">
+      <c r="N53" s="7">
         <f t="shared" si="41"/>
         <v>-0.80964914709688807</v>
       </c>
-      <c r="O53" s="9">
+      <c r="O53" s="7">
         <f t="shared" si="41"/>
         <v>-1.3783908963163696</v>
       </c>
-      <c r="P53" s="9">
+      <c r="P53" s="7">
         <f t="shared" si="41"/>
         <v>-1.2820410770867725</v>
       </c>
-      <c r="Q53" s="9">
+      <c r="Q53" s="7">
         <f t="shared" si="41"/>
         <v>-0.47454957187682678</v>
       </c>
+      <c r="R53" s="8">
+        <f>MAX(B51:L51)</f>
+        <v>1.5501200098354908</v>
+      </c>
+      <c r="S53" s="8">
+        <f>AVERAGE(B51:L51)</f>
+        <v>0.45420134407797919</v>
+      </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B54" s="9">
+      <c r="B54" s="7">
         <f t="shared" si="41"/>
         <v>-1.2774124929719315</v>
       </c>
-      <c r="C54" s="9">
+      <c r="C54" s="7">
         <f t="shared" si="41"/>
         <v>-1.3222373586384988</v>
       </c>
-      <c r="D54" s="9">
+      <c r="D54" s="7">
         <f t="shared" si="41"/>
         <v>-1.3313460003052142</v>
       </c>
-      <c r="E54" s="9">
+      <c r="E54" s="7">
         <f t="shared" si="41"/>
         <v>-1.3639675329842595</v>
       </c>
-      <c r="F54" s="9">
+      <c r="F54" s="7">
         <f t="shared" si="41"/>
         <v>-1.3786739003152082</v>
       </c>
-      <c r="G54" s="9">
+      <c r="G54" s="7">
         <f t="shared" si="41"/>
         <v>-1.0648977406922207</v>
       </c>
-      <c r="H54" s="9">
+      <c r="H54" s="7">
         <f t="shared" si="41"/>
         <v>-1.4328389945321076</v>
       </c>
-      <c r="I54" s="9">
+      <c r="I54" s="7">
         <f t="shared" si="41"/>
         <v>-1.4913013470582166</v>
       </c>
-      <c r="J54" s="9">
+      <c r="J54" s="7">
         <f t="shared" si="41"/>
         <v>-1.4606517551926532</v>
       </c>
-      <c r="K54" s="9">
+      <c r="K54" s="7">
         <f t="shared" si="41"/>
         <v>-1.3792349730687858</v>
       </c>
-      <c r="L54" s="9">
+      <c r="L54" s="7">
         <f t="shared" si="41"/>
         <v>-1.4905901944776432</v>
       </c>
-      <c r="M54" s="9">
+      <c r="M54" s="7">
         <f t="shared" si="41"/>
         <v>-0.96465660937476516</v>
       </c>
-      <c r="N54" s="9">
+      <c r="N54" s="7">
         <f t="shared" si="41"/>
         <v>-1.8725521749741234</v>
       </c>
-      <c r="O54" s="9">
+      <c r="O54" s="7">
         <f t="shared" si="41"/>
         <v>-1.6151614152258986</v>
       </c>
-      <c r="P54" s="9">
+      <c r="P54" s="7">
         <f t="shared" si="41"/>
         <v>-3.5810560421586914</v>
       </c>
-      <c r="Q54" s="9">
+      <c r="Q54" s="7">
         <f t="shared" si="41"/>
         <v>-1.3793996487666671</v>
       </c>

</xml_diff>